<commit_message>
[ADD] invoice_codes and glns_codes added to xlsx template for massive load
</commit_message>
<xml_diff>
--- a/rvc/static/xls/Plantilla_Beneficiarias_Identificacion.xlsx
+++ b/rvc/static/xls/Plantilla_Beneficiarias_Identificacion.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Nit Beneficiaria</t>
   </si>
@@ -28,7 +28,13 @@
     <t xml:space="preserve">Nit Halonadora</t>
   </si>
   <si>
-    <t xml:space="preserve">Cantidad de Códigos</t>
+    <t xml:space="preserve">Cantidad de Códigos Producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cantidad de Códigos GLN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cantidad de Códigos Recaudo</t>
   </si>
   <si>
     <t xml:space="preserve">Nombre Contacto</t>
@@ -154,16 +160,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:G2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:G2"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:I2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:I2"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="Nit Beneficiaria"/>
     <tableColumn id="2" name="Nit Halonadora"/>
-    <tableColumn id="3" name="Cantidad de Códigos"/>
-    <tableColumn id="4" name="Nombre Contacto"/>
-    <tableColumn id="5" name="Correo Contacto"/>
-    <tableColumn id="6" name="Teléfono Contacto"/>
-    <tableColumn id="7" name="Cargo Contacto"/>
+    <tableColumn id="3" name="Cantidad de Códigos Producto"/>
+    <tableColumn id="4" name="Cantidad de Códigos GLN"/>
+    <tableColumn id="5" name="Cantidad de Códigos Recaudo"/>
+    <tableColumn id="6" name="Nombre Contacto"/>
+    <tableColumn id="7" name="Correo Contacto"/>
+    <tableColumn id="8" name="Teléfono Contacto"/>
+    <tableColumn id="9" name="Cargo Contacto"/>
   </tableColumns>
 </table>
 </file>
@@ -173,23 +181,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="28.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -214,8 +224,14 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>